<commit_message>
made changes to client
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/data/CreateUserData.xlsx
+++ b/src/main/java/com/qa/data/CreateUserData.xlsx
@@ -3,18 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkshank\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14880" windowHeight="5955"/>
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="1" r:id="rId1"/>
+    <sheet name="GetUserDetails" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:T17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,22 +47,22 @@
     <t>inactive</t>
   </si>
   <si>
-    <t>Tom</t>
-  </si>
-  <si>
     <t>Hanks</t>
   </si>
   <si>
-    <t>tomhanks@zmail.com</t>
-  </si>
-  <si>
-    <t>john</t>
-  </si>
-  <si>
     <t>swan</t>
   </si>
   <si>
-    <t>johnswam@zmail.com</t>
+    <t>Tom3</t>
+  </si>
+  <si>
+    <t>john4</t>
+  </si>
+  <si>
+    <t>tomhanks3@zmail.com</t>
+  </si>
+  <si>
+    <t>johnswam4@zmail.com</t>
   </si>
 </sst>
 </file>
@@ -397,10 +394,13 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="46.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -421,16 +421,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -441,7 +441,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -460,4 +460,16 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>